<commit_message>
added shield and boots
</commit_message>
<xml_diff>
--- a/data/global/excel/CORRUPTION LISTS.xlsx
+++ b/data/global/excel/CORRUPTION LISTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rucdk-my.sharepoint.com/personal/magnuha_ruc_dk/Documents/Documents/GitHub/d2-nd-jexmod/data/global/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7A0B43B-A1F2-4CA8-B35B-BA590805E885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{B7A0B43B-A1F2-4CA8-B35B-BA590805E885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72BDDFE7-BBD6-4001-8694-EAD1306DB2C2}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E3FD12B3-9020-44F4-A3E1-112F3CF80D13}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="54">
   <si>
     <t>Corruption Tracker</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>Belt + Glyph -&gt; Corrupted Belt With Useful Stat</t>
+  </si>
+  <si>
+    <t>shield,nor,nos</t>
+  </si>
+  <si>
+    <t>shield,hiq,nos</t>
+  </si>
+  <si>
+    <t>shield,nos</t>
+  </si>
+  <si>
+    <t>shield,sock</t>
   </si>
 </sst>
 </file>
@@ -535,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A09F29B-EC61-4D8E-B843-508314F6E461}">
-  <dimension ref="A1:AH64"/>
+  <dimension ref="A1:AH92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -850,19 +862,19 @@
         <v>24</v>
       </c>
       <c r="K14" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="Q14" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="W14" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="AC14" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AH14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.55000000000000004">
@@ -873,19 +885,19 @@
         <v>24</v>
       </c>
       <c r="K15" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="Q15" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="W15" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="AC15" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="AH15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.55000000000000004">
@@ -896,19 +908,19 @@
         <v>24</v>
       </c>
       <c r="K16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AC16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AH16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.55000000000000004">
@@ -919,19 +931,19 @@
         <v>24</v>
       </c>
       <c r="K17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AC17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AH17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.55000000000000004">
@@ -1148,21 +1160,6 @@
       <c r="F27" t="s">
         <v>24</v>
       </c>
-      <c r="K27" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>30</v>
-      </c>
-      <c r="W27" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
@@ -1171,21 +1168,6 @@
       <c r="F28" t="s">
         <v>24</v>
       </c>
-      <c r="K28" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>30</v>
-      </c>
-      <c r="W28" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH28" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
@@ -1218,24 +1200,33 @@
       <c r="F32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>10</v>
       </c>
       <c r="F33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>10</v>
       </c>
       <c r="F34" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1243,236 +1234,441 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+      <c r="L36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>5</v>
       </c>
       <c r="F37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+      <c r="L37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>22</v>
+      </c>
+      <c r="L38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>11</v>
       </c>
       <c r="F40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+      <c r="L40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>10</v>
       </c>
       <c r="F41" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>10</v>
       </c>
       <c r="F42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>10</v>
       </c>
       <c r="F43" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>10</v>
       </c>
       <c r="F44" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>10</v>
       </c>
       <c r="F45" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>10</v>
       </c>
       <c r="F46" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>10</v>
       </c>
       <c r="F47" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>10</v>
       </c>
       <c r="F48" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>10</v>
       </c>
       <c r="F49" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>10</v>
       </c>
       <c r="F50" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>18</v>
+      </c>
+      <c r="L50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>6</v>
       </c>
       <c r="F51" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+      <c r="L51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>23</v>
+      </c>
+      <c r="L52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>11</v>
       </c>
       <c r="F53" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>10</v>
       </c>
       <c r="F54" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>10</v>
       </c>
       <c r="F55" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>10</v>
       </c>
       <c r="F56" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>10</v>
       </c>
       <c r="F57" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>10</v>
       </c>
       <c r="F58" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L58" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>10</v>
       </c>
       <c r="F59" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>10</v>
       </c>
       <c r="F60" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L60" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>10</v>
       </c>
       <c r="F61" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L61" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>10</v>
       </c>
       <c r="F62" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>10</v>
       </c>
-      <c r="F63" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="L63" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>10</v>
       </c>
-      <c r="F64" t="s">
-        <v>24</v>
+      <c r="L64" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L67" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L68" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L69" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="70" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L70" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L71" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L72" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="73" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L73" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="74" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L74" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L75" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="76" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L76" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L77" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L78" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="79" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L79" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L81" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L82" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="83" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L83" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="84" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L84" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="85" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L85" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="86" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L86" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L87" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="88" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L88" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="89" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L89" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L90" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="91" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L91" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="92" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L92" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>